<commit_message>
correct the axioms needed to also have "acylation" as inferred parent of  "univalent carboacylation"
</commit_message>
<xml_diff>
--- a/MOP_vs_RXNO.xlsx
+++ b/MOP_vs_RXNO.xlsx
@@ -22064,14 +22064,58 @@
     <t>Colins comment</t>
   </si>
   <si>
-    <t xml:space="preserve">seems to me that the RXNO version was edit second; I would suggest to use MOPs version with the parent class "univalent carboacylation" but add the "has_participant some 'formyl group'" as subclass of axiom to this; wrt the RXNO verison parent "acylation" - we would get "univalent carboacylation" to be an inferred child of "acylation" once we'd assert "acylation" to be equivalent to 'formation of covalent bond with carbon centre' and has_participant some 'acyl group'; but the latter would be part of the equivalent to issue that I'd rather want to tackle later. </t>
+    <r>
+      <t xml:space="preserve">seems to me that the RXNO version was edit second; I would suggest to use MOPs version with the parent class "univalent carboacylation" but add the "has_participant some 'formyl group'" as subclass of axiom to this; wrt the RXNO verison parent "acylation" - we would get "univalent carboacylation" to be an inferred child of "acylation" once we'd assert "acylation" to be equivalent to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'formation of covalent bond with carbon centre' and has_participant some 'acyl group'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as well as adding the SubclassOf axiom</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> has_participant some 'carboacyl group' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">to "univalent carboacylation" ; but the latter would be part of the equivalent to issue that I'd rather want to tackle later. </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -22081,6 +22125,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -22803,7 +22855,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22902,7 +22954,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="300" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
#27 reconcile: MOP:0000339, MOP:0000364, MOP:0000369, MOP:0000410, MOP:0000411
</commit_message>
<xml_diff>
--- a/MOP_vs_RXNO.xlsx
+++ b/MOP_vs_RXNO.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11093" uniqueCount="7343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11098" uniqueCount="7345">
   <si>
     <t>ID</t>
   </si>
@@ -22110,6 +22110,35 @@
       <t xml:space="preserve">to "univalent carboacylation" ; but the latter would be part of the equivalent to issue that I'd rather want to tackle later. </t>
     </r>
   </si>
+  <si>
+    <t>the one in RXNO can savely be deleted</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">add subclassOf axiom </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">has_participant some 'aryl group' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to MOP version</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -22140,7 +22169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -22150,6 +22179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -22476,7 +22511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -22546,6 +22581,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -22854,8 +22897,8 @@
   <dimension ref="A1:H3631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="2" topLeftCell="A403" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C421" sqref="C421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22866,7 +22909,7 @@
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.85546875" customWidth="1"/>
     <col min="6" max="6" width="46.42578125" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" style="35" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" style="35" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22954,7 +22997,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -27581,7 +27624,7 @@
       <c r="E336" s="5"/>
       <c r="F336" s="16"/>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A337" s="5" t="s">
         <v>681</v>
       </c>
@@ -27595,7 +27638,7 @@
       <c r="E337" s="5"/>
       <c r="F337" s="16"/>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A338" s="5" t="s">
         <v>683</v>
       </c>
@@ -27609,7 +27652,7 @@
       <c r="E338" s="5"/>
       <c r="F338" s="16"/>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A339" s="5" t="s">
         <v>686</v>
       </c>
@@ -27623,7 +27666,7 @@
       <c r="E339" s="5"/>
       <c r="F339" s="16"/>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A340" s="5" t="s">
         <v>688</v>
       </c>
@@ -27637,7 +27680,7 @@
       <c r="E340" s="5"/>
       <c r="F340" s="16"/>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A341" s="5" t="s">
         <v>690</v>
       </c>
@@ -27651,27 +27694,30 @@
       <c r="E341" s="5"/>
       <c r="F341" s="16"/>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A342" s="5" t="s">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A342" s="39" t="s">
         <v>692</v>
       </c>
-      <c r="B342" s="5" t="s">
+      <c r="B342" s="39" t="s">
         <v>693</v>
       </c>
-      <c r="C342" s="23" t="s">
+      <c r="C342" s="40" t="s">
         <v>694</v>
       </c>
-      <c r="D342" s="17" t="s">
+      <c r="D342" s="41" t="s">
         <v>692</v>
       </c>
-      <c r="E342" s="5" t="s">
+      <c r="E342" s="39" t="s">
         <v>693</v>
       </c>
-      <c r="F342" s="16" t="s">
+      <c r="F342" s="42" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G342" s="35" t="s">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A343" s="5" t="s">
         <v>696</v>
       </c>
@@ -27685,7 +27731,7 @@
       <c r="E343" s="5"/>
       <c r="F343" s="16"/>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A344" s="5" t="s">
         <v>698</v>
       </c>
@@ -27699,7 +27745,7 @@
       <c r="E344" s="5"/>
       <c r="F344" s="16"/>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A345" s="5" t="s">
         <v>700</v>
       </c>
@@ -27713,7 +27759,7 @@
       <c r="E345" s="5"/>
       <c r="F345" s="16"/>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A346" s="5" t="s">
         <v>702</v>
       </c>
@@ -27727,7 +27773,7 @@
       <c r="E346" s="5"/>
       <c r="F346" s="16"/>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A347" s="5" t="s">
         <v>704</v>
       </c>
@@ -27741,7 +27787,7 @@
       <c r="E347" s="5"/>
       <c r="F347" s="16"/>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A348" s="5" t="s">
         <v>707</v>
       </c>
@@ -27755,7 +27801,7 @@
       <c r="E348" s="5"/>
       <c r="F348" s="16"/>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="5" t="s">
         <v>710</v>
       </c>
@@ -27769,7 +27815,7 @@
       <c r="E349" s="5"/>
       <c r="F349" s="16"/>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A350" s="5" t="s">
         <v>712</v>
       </c>
@@ -27783,7 +27829,7 @@
       <c r="E350" s="5"/>
       <c r="F350" s="16"/>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A351" s="5" t="s">
         <v>715</v>
       </c>
@@ -27797,7 +27843,7 @@
       <c r="E351" s="5"/>
       <c r="F351" s="16"/>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A352" s="5" t="s">
         <v>717</v>
       </c>
@@ -27811,7 +27857,7 @@
       <c r="E352" s="5"/>
       <c r="F352" s="16"/>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A353" s="5" t="s">
         <v>720</v>
       </c>
@@ -27825,7 +27871,7 @@
       <c r="E353" s="5"/>
       <c r="F353" s="16"/>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A354" s="5" t="s">
         <v>723</v>
       </c>
@@ -27839,7 +27885,7 @@
       <c r="E354" s="5"/>
       <c r="F354" s="16"/>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A355" s="5" t="s">
         <v>726</v>
       </c>
@@ -27853,7 +27899,7 @@
       <c r="E355" s="5"/>
       <c r="F355" s="16"/>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A356" s="5" t="s">
         <v>728</v>
       </c>
@@ -27867,7 +27913,7 @@
       <c r="E356" s="5"/>
       <c r="F356" s="16"/>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A357" s="5" t="s">
         <v>730</v>
       </c>
@@ -27881,7 +27927,7 @@
       <c r="E357" s="5"/>
       <c r="F357" s="16"/>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A358" s="5" t="s">
         <v>732</v>
       </c>
@@ -27895,7 +27941,7 @@
       <c r="E358" s="5"/>
       <c r="F358" s="16"/>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A359" s="5" t="s">
         <v>734</v>
       </c>
@@ -27909,7 +27955,7 @@
       <c r="E359" s="5"/>
       <c r="F359" s="16"/>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A360" s="5" t="s">
         <v>736</v>
       </c>
@@ -27923,7 +27969,7 @@
       <c r="E360" s="5"/>
       <c r="F360" s="16"/>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A361" s="5" t="s">
         <v>738</v>
       </c>
@@ -27937,7 +27983,7 @@
       <c r="E361" s="5"/>
       <c r="F361" s="16"/>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A362" s="5" t="s">
         <v>740</v>
       </c>
@@ -27951,7 +27997,7 @@
       <c r="E362" s="5"/>
       <c r="F362" s="16"/>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A363" s="5" t="s">
         <v>742</v>
       </c>
@@ -27965,7 +28011,7 @@
       <c r="E363" s="5"/>
       <c r="F363" s="16"/>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A364" s="5" t="s">
         <v>744</v>
       </c>
@@ -27979,7 +28025,7 @@
       <c r="E364" s="5"/>
       <c r="F364" s="16"/>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" s="5" t="s">
         <v>746</v>
       </c>
@@ -27993,7 +28039,7 @@
       <c r="E365" s="5"/>
       <c r="F365" s="16"/>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A366" s="5" t="s">
         <v>749</v>
       </c>
@@ -28007,27 +28053,30 @@
       <c r="E366" s="5"/>
       <c r="F366" s="16"/>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A367" s="5" t="s">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A367" s="39" t="s">
         <v>752</v>
       </c>
-      <c r="B367" s="5" t="s">
+      <c r="B367" s="39" t="s">
         <v>753</v>
       </c>
-      <c r="C367" s="23" t="s">
+      <c r="C367" s="40" t="s">
         <v>751</v>
       </c>
-      <c r="D367" s="17" t="s">
+      <c r="D367" s="41" t="s">
         <v>752</v>
       </c>
-      <c r="E367" s="5" t="s">
+      <c r="E367" s="39" t="s">
         <v>753</v>
       </c>
-      <c r="F367" s="16" t="s">
+      <c r="F367" s="42" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G367" s="35" t="s">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" s="5" t="s">
         <v>754</v>
       </c>
@@ -28041,7 +28090,7 @@
       <c r="E368" s="5"/>
       <c r="F368" s="16"/>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A369" s="5" t="s">
         <v>756</v>
       </c>
@@ -28055,7 +28104,7 @@
       <c r="E369" s="5"/>
       <c r="F369" s="16"/>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A370" s="5" t="s">
         <v>758</v>
       </c>
@@ -28069,7 +28118,7 @@
       <c r="E370" s="5"/>
       <c r="F370" s="16"/>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" s="5" t="s">
         <v>761</v>
       </c>
@@ -28083,27 +28132,30 @@
       <c r="E371" s="5"/>
       <c r="F371" s="16"/>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A372" s="5" t="s">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A372" s="39" t="s">
         <v>763</v>
       </c>
-      <c r="B372" s="5" t="s">
+      <c r="B372" s="39" t="s">
         <v>751</v>
       </c>
-      <c r="C372" s="23" t="s">
+      <c r="C372" s="40" t="s">
         <v>764</v>
       </c>
-      <c r="D372" s="17" t="s">
+      <c r="D372" s="41" t="s">
         <v>763</v>
       </c>
-      <c r="E372" s="5" t="s">
+      <c r="E372" s="39" t="s">
         <v>751</v>
       </c>
-      <c r="F372" s="16" t="s">
+      <c r="F372" s="42" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G372" s="35" t="s">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A373" s="5" t="s">
         <v>765</v>
       </c>
@@ -28117,7 +28169,7 @@
       <c r="E373" s="5"/>
       <c r="F373" s="16"/>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A374" s="5" t="s">
         <v>767</v>
       </c>
@@ -28131,7 +28183,7 @@
       <c r="E374" s="5"/>
       <c r="F374" s="16"/>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A375" s="5" t="s">
         <v>769</v>
       </c>
@@ -28145,7 +28197,7 @@
       <c r="E375" s="5"/>
       <c r="F375" s="16"/>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A376" s="5" t="s">
         <v>771</v>
       </c>
@@ -28159,7 +28211,7 @@
       <c r="E376" s="5"/>
       <c r="F376" s="16"/>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A377" s="5" t="s">
         <v>773</v>
       </c>
@@ -28173,7 +28225,7 @@
       <c r="E377" s="5"/>
       <c r="F377" s="16"/>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A378" s="5" t="s">
         <v>775</v>
       </c>
@@ -28187,7 +28239,7 @@
       <c r="E378" s="5"/>
       <c r="F378" s="16"/>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A379" s="5" t="s">
         <v>777</v>
       </c>
@@ -28201,7 +28253,7 @@
       <c r="E379" s="5"/>
       <c r="F379" s="16"/>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A380" s="5" t="s">
         <v>779</v>
       </c>
@@ -28215,7 +28267,7 @@
       <c r="E380" s="5"/>
       <c r="F380" s="16"/>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A381" s="5" t="s">
         <v>781</v>
       </c>
@@ -28229,7 +28281,7 @@
       <c r="E381" s="5"/>
       <c r="F381" s="16"/>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A382" s="5" t="s">
         <v>783</v>
       </c>
@@ -28243,7 +28295,7 @@
       <c r="E382" s="5"/>
       <c r="F382" s="16"/>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A383" s="5" t="s">
         <v>785</v>
       </c>
@@ -28257,7 +28309,7 @@
       <c r="E383" s="5"/>
       <c r="F383" s="16"/>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A384" s="5" t="s">
         <v>787</v>
       </c>
@@ -28495,7 +28547,7 @@
       <c r="E400" s="5"/>
       <c r="F400" s="16"/>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" s="5" t="s">
         <v>821</v>
       </c>
@@ -28509,7 +28561,7 @@
       <c r="E401" s="5"/>
       <c r="F401" s="16"/>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="5" t="s">
         <v>823</v>
       </c>
@@ -28523,7 +28575,7 @@
       <c r="E402" s="5"/>
       <c r="F402" s="16"/>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" s="5" t="s">
         <v>825</v>
       </c>
@@ -28537,7 +28589,7 @@
       <c r="E403" s="5"/>
       <c r="F403" s="16"/>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A404" s="5" t="s">
         <v>827</v>
       </c>
@@ -28551,7 +28603,7 @@
       <c r="E404" s="5"/>
       <c r="F404" s="16"/>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A405" s="5" t="s">
         <v>829</v>
       </c>
@@ -28565,7 +28617,7 @@
       <c r="E405" s="5"/>
       <c r="F405" s="16"/>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A406" s="5" t="s">
         <v>831</v>
       </c>
@@ -28579,7 +28631,7 @@
       <c r="E406" s="5"/>
       <c r="F406" s="16"/>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A407" s="5" t="s">
         <v>833</v>
       </c>
@@ -28593,7 +28645,7 @@
       <c r="E407" s="5"/>
       <c r="F407" s="16"/>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A408" s="5" t="s">
         <v>835</v>
       </c>
@@ -28607,7 +28659,7 @@
       <c r="E408" s="5"/>
       <c r="F408" s="16"/>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A409" s="5" t="s">
         <v>837</v>
       </c>
@@ -28621,7 +28673,7 @@
       <c r="E409" s="5"/>
       <c r="F409" s="16"/>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A410" s="5" t="s">
         <v>839</v>
       </c>
@@ -28635,7 +28687,7 @@
       <c r="E410" s="5"/>
       <c r="F410" s="16"/>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" s="5" t="s">
         <v>841</v>
       </c>
@@ -28649,7 +28701,7 @@
       <c r="E411" s="5"/>
       <c r="F411" s="16"/>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A412" s="5" t="s">
         <v>843</v>
       </c>
@@ -28663,47 +28715,53 @@
       <c r="E412" s="5"/>
       <c r="F412" s="16"/>
     </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A413" s="5" t="s">
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A413" s="39" t="s">
         <v>845</v>
       </c>
-      <c r="B413" s="5" t="s">
+      <c r="B413" s="39" t="s">
         <v>764</v>
       </c>
-      <c r="C413" s="23" t="s">
+      <c r="C413" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="D413" s="17" t="s">
+      <c r="D413" s="41" t="s">
         <v>845</v>
       </c>
-      <c r="E413" s="5" t="s">
+      <c r="E413" s="39" t="s">
         <v>764</v>
       </c>
-      <c r="F413" s="16" t="s">
+      <c r="F413" s="42" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A414" s="5" t="s">
+      <c r="G413" s="35" t="s">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A414" s="43" t="s">
         <v>846</v>
       </c>
-      <c r="B414" s="5" t="s">
+      <c r="B414" s="43" t="s">
         <v>847</v>
       </c>
-      <c r="C414" s="23" t="s">
+      <c r="C414" s="36" t="s">
         <v>764</v>
       </c>
-      <c r="D414" s="17" t="s">
+      <c r="D414" s="44" t="s">
         <v>846</v>
       </c>
-      <c r="E414" s="5" t="s">
+      <c r="E414" s="43" t="s">
         <v>847</v>
       </c>
-      <c r="F414" s="16" t="s">
+      <c r="F414" s="37" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G414" s="35" t="s">
+        <v>7344</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="5" t="s">
         <v>849</v>
       </c>
@@ -28717,7 +28775,7 @@
       <c r="E415" s="5"/>
       <c r="F415" s="16"/>
     </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416" s="5" t="s">
         <v>851</v>
       </c>

</xml_diff>

<commit_message>
#27 reconciling: MOP:0000422, MOP:0000458, MOP:0000479, MOP:0000539
</commit_message>
<xml_diff>
--- a/MOP_vs_RXNO.xlsx
+++ b/MOP_vs_RXNO.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11098" uniqueCount="7345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11102" uniqueCount="7348">
   <si>
     <t>ID</t>
   </si>
@@ -22138,6 +22138,15 @@
       </rPr>
       <t>to MOP version</t>
     </r>
+  </si>
+  <si>
+    <t>use parent of MOP version as it is more specific, thus the RXNO version can be discarded</t>
+  </si>
+  <si>
+    <t>delete equivalentTo axiom in MOP version and subsume under "organylation" there analog the the RXNO version before discarding in RXNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use the MOP version's parent as it's more specific but copy the rdfs:comment </t>
   </si>
 </sst>
 </file>
@@ -22511,7 +22520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -22572,8 +22581,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -22589,6 +22596,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -22897,8 +22907,8 @@
   <dimension ref="A1:H3631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A403" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C421" sqref="C421"/>
+      <pane ySplit="2" topLeftCell="A518" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D545" sqref="D545"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22909,7 +22919,7 @@
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.85546875" customWidth="1"/>
     <col min="6" max="6" width="46.42578125" customWidth="1"/>
-    <col min="7" max="7" width="54.85546875" style="35" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" style="36" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22966,7 +22976,7 @@
       <c r="D3" s="20"/>
       <c r="E3" s="6"/>
       <c r="F3" s="15"/>
-      <c r="G3" s="34"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -23004,7 +23014,7 @@
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="17" t="s">
@@ -23013,10 +23023,10 @@
       <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="36" t="s">
         <v>7342</v>
       </c>
     </row>
@@ -27695,25 +27705,25 @@
       <c r="F341" s="16"/>
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A342" s="39" t="s">
+      <c r="A342" s="37" t="s">
         <v>692</v>
       </c>
-      <c r="B342" s="39" t="s">
+      <c r="B342" s="37" t="s">
         <v>693</v>
       </c>
-      <c r="C342" s="40" t="s">
+      <c r="C342" s="38" t="s">
         <v>694</v>
       </c>
-      <c r="D342" s="41" t="s">
+      <c r="D342" s="39" t="s">
         <v>692</v>
       </c>
-      <c r="E342" s="39" t="s">
+      <c r="E342" s="37" t="s">
         <v>693</v>
       </c>
-      <c r="F342" s="42" t="s">
+      <c r="F342" s="40" t="s">
         <v>695</v>
       </c>
-      <c r="G342" s="35" t="s">
+      <c r="G342" s="36" t="s">
         <v>7343</v>
       </c>
     </row>
@@ -28054,25 +28064,25 @@
       <c r="F366" s="16"/>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A367" s="39" t="s">
+      <c r="A367" s="37" t="s">
         <v>752</v>
       </c>
-      <c r="B367" s="39" t="s">
+      <c r="B367" s="37" t="s">
         <v>753</v>
       </c>
-      <c r="C367" s="40" t="s">
+      <c r="C367" s="38" t="s">
         <v>751</v>
       </c>
-      <c r="D367" s="41" t="s">
+      <c r="D367" s="39" t="s">
         <v>752</v>
       </c>
-      <c r="E367" s="39" t="s">
+      <c r="E367" s="37" t="s">
         <v>753</v>
       </c>
-      <c r="F367" s="42" t="s">
+      <c r="F367" s="40" t="s">
         <v>751</v>
       </c>
-      <c r="G367" s="35" t="s">
+      <c r="G367" s="36" t="s">
         <v>7343</v>
       </c>
     </row>
@@ -28133,25 +28143,25 @@
       <c r="F371" s="16"/>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A372" s="39" t="s">
+      <c r="A372" s="37" t="s">
         <v>763</v>
       </c>
-      <c r="B372" s="39" t="s">
+      <c r="B372" s="37" t="s">
         <v>751</v>
       </c>
-      <c r="C372" s="40" t="s">
+      <c r="C372" s="38" t="s">
         <v>764</v>
       </c>
-      <c r="D372" s="41" t="s">
+      <c r="D372" s="39" t="s">
         <v>763</v>
       </c>
-      <c r="E372" s="39" t="s">
+      <c r="E372" s="37" t="s">
         <v>751</v>
       </c>
-      <c r="F372" s="42" t="s">
+      <c r="F372" s="40" t="s">
         <v>764</v>
       </c>
-      <c r="G372" s="35" t="s">
+      <c r="G372" s="36" t="s">
         <v>7343</v>
       </c>
     </row>
@@ -28716,48 +28726,48 @@
       <c r="F412" s="16"/>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A413" s="39" t="s">
+      <c r="A413" s="37" t="s">
         <v>845</v>
       </c>
-      <c r="B413" s="39" t="s">
+      <c r="B413" s="37" t="s">
         <v>764</v>
       </c>
-      <c r="C413" s="40" t="s">
+      <c r="C413" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D413" s="41" t="s">
+      <c r="D413" s="39" t="s">
         <v>845</v>
       </c>
-      <c r="E413" s="39" t="s">
+      <c r="E413" s="37" t="s">
         <v>764</v>
       </c>
-      <c r="F413" s="42" t="s">
+      <c r="F413" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="G413" s="35" t="s">
+      <c r="G413" s="36" t="s">
         <v>7343</v>
       </c>
     </row>
-    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A414" s="43" t="s">
+    <row r="414" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A414" s="41" t="s">
         <v>846</v>
       </c>
-      <c r="B414" s="43" t="s">
+      <c r="B414" s="41" t="s">
         <v>847</v>
       </c>
-      <c r="C414" s="36" t="s">
+      <c r="C414" s="34" t="s">
         <v>764</v>
       </c>
-      <c r="D414" s="44" t="s">
+      <c r="D414" s="42" t="s">
         <v>846</v>
       </c>
-      <c r="E414" s="43" t="s">
+      <c r="E414" s="41" t="s">
         <v>847</v>
       </c>
-      <c r="F414" s="37" t="s">
+      <c r="F414" s="35" t="s">
         <v>848</v>
       </c>
-      <c r="G414" s="35" t="s">
+      <c r="G414" s="36" t="s">
         <v>7344</v>
       </c>
     </row>
@@ -28789,7 +28799,7 @@
       <c r="E416" s="5"/>
       <c r="F416" s="16"/>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A417" s="5" t="s">
         <v>853</v>
       </c>
@@ -28803,7 +28813,7 @@
       <c r="E417" s="5"/>
       <c r="F417" s="16"/>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A418" s="5" t="s">
         <v>855</v>
       </c>
@@ -28817,7 +28827,7 @@
       <c r="E418" s="5"/>
       <c r="F418" s="16"/>
     </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A419" s="5" t="s">
         <v>857</v>
       </c>
@@ -28831,7 +28841,7 @@
       <c r="E419" s="5"/>
       <c r="F419" s="16"/>
     </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420" s="5" t="s">
         <v>859</v>
       </c>
@@ -28845,7 +28855,7 @@
       <c r="E420" s="5"/>
       <c r="F420" s="16"/>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A421" s="5" t="s">
         <v>861</v>
       </c>
@@ -28859,7 +28869,7 @@
       <c r="E421" s="5"/>
       <c r="F421" s="16"/>
     </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422" s="5" t="s">
         <v>863</v>
       </c>
@@ -28873,7 +28883,7 @@
       <c r="E422" s="5"/>
       <c r="F422" s="16"/>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A423" s="5" t="s">
         <v>865</v>
       </c>
@@ -28887,7 +28897,7 @@
       <c r="E423" s="5"/>
       <c r="F423" s="16"/>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A424" s="5" t="s">
         <v>867</v>
       </c>
@@ -28901,27 +28911,30 @@
       <c r="E424" s="5"/>
       <c r="F424" s="16"/>
     </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A425" s="5" t="s">
+    <row r="425" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A425" s="41" t="s">
         <v>869</v>
       </c>
-      <c r="B425" s="5" t="s">
+      <c r="B425" s="41" t="s">
         <v>870</v>
       </c>
-      <c r="C425" s="23" t="s">
+      <c r="C425" s="34" t="s">
         <v>866</v>
       </c>
-      <c r="D425" s="17" t="s">
+      <c r="D425" s="42" t="s">
         <v>869</v>
       </c>
-      <c r="E425" s="5" t="s">
+      <c r="E425" s="41" t="s">
         <v>870</v>
       </c>
-      <c r="F425" s="16" t="s">
+      <c r="F425" s="35" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G425" s="36" t="s">
+        <v>7345</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A426" s="5" t="s">
         <v>871</v>
       </c>
@@ -28935,7 +28948,7 @@
       <c r="E426" s="5"/>
       <c r="F426" s="16"/>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A427" s="5" t="s">
         <v>873</v>
       </c>
@@ -28949,7 +28962,7 @@
       <c r="E427" s="5"/>
       <c r="F427" s="16"/>
     </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A428" s="5" t="s">
         <v>875</v>
       </c>
@@ -28963,7 +28976,7 @@
       <c r="E428" s="5"/>
       <c r="F428" s="16"/>
     </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A429" s="5" t="s">
         <v>877</v>
       </c>
@@ -28977,7 +28990,7 @@
       <c r="E429" s="5"/>
       <c r="F429" s="16"/>
     </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A430" s="5" t="s">
         <v>879</v>
       </c>
@@ -28987,7 +29000,7 @@
       <c r="E430" s="5"/>
       <c r="F430" s="16"/>
     </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A431" s="5" t="s">
         <v>880</v>
       </c>
@@ -29001,7 +29014,7 @@
       <c r="E431" s="5"/>
       <c r="F431" s="16"/>
     </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A432" s="5" t="s">
         <v>882</v>
       </c>
@@ -29239,7 +29252,7 @@
       <c r="E448" s="5"/>
       <c r="F448" s="16"/>
     </row>
-    <row r="449" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A449" s="5" t="s">
         <v>916</v>
       </c>
@@ -29253,7 +29266,7 @@
       <c r="E449" s="5"/>
       <c r="F449" s="16"/>
     </row>
-    <row r="450" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A450" s="5" t="s">
         <v>919</v>
       </c>
@@ -29267,7 +29280,7 @@
       <c r="E450" s="5"/>
       <c r="F450" s="16"/>
     </row>
-    <row r="451" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A451" s="5" t="s">
         <v>921</v>
       </c>
@@ -29281,7 +29294,7 @@
       <c r="E451" s="5"/>
       <c r="F451" s="16"/>
     </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A452" s="5" t="s">
         <v>923</v>
       </c>
@@ -29295,7 +29308,7 @@
       <c r="E452" s="5"/>
       <c r="F452" s="16"/>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A453" s="5" t="s">
         <v>925</v>
       </c>
@@ -29309,7 +29322,7 @@
       <c r="E453" s="5"/>
       <c r="F453" s="16"/>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A454" s="5" t="s">
         <v>927</v>
       </c>
@@ -29323,7 +29336,7 @@
       <c r="E454" s="5"/>
       <c r="F454" s="16"/>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A455" s="5" t="s">
         <v>929</v>
       </c>
@@ -29337,7 +29350,7 @@
       <c r="E455" s="5"/>
       <c r="F455" s="16"/>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A456" s="5" t="s">
         <v>932</v>
       </c>
@@ -29351,7 +29364,7 @@
       <c r="E456" s="5"/>
       <c r="F456" s="16"/>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" s="5" t="s">
         <v>934</v>
       </c>
@@ -29365,7 +29378,7 @@
       <c r="E457" s="5"/>
       <c r="F457" s="16"/>
     </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A458" s="5" t="s">
         <v>936</v>
       </c>
@@ -29379,7 +29392,7 @@
       <c r="E458" s="5"/>
       <c r="F458" s="16"/>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A459" s="5" t="s">
         <v>938</v>
       </c>
@@ -29393,7 +29406,7 @@
       <c r="E459" s="5"/>
       <c r="F459" s="16"/>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460" s="5" t="s">
         <v>940</v>
       </c>
@@ -29407,27 +29420,30 @@
       <c r="E460" s="5"/>
       <c r="F460" s="16"/>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A461" s="5" t="s">
+    <row r="461" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A461" s="41" t="s">
         <v>942</v>
       </c>
-      <c r="B461" s="5" t="s">
+      <c r="B461" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C461" s="23" t="s">
+      <c r="C461" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D461" s="17" t="s">
+      <c r="D461" s="42" t="s">
         <v>942</v>
       </c>
-      <c r="E461" s="5" t="s">
+      <c r="E461" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="F461" s="16" t="s">
+      <c r="F461" s="35" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G461" s="36" t="s">
+        <v>7345</v>
+      </c>
+    </row>
+    <row r="462" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A462" s="5" t="s">
         <v>943</v>
       </c>
@@ -29441,7 +29457,7 @@
       <c r="E462" s="5"/>
       <c r="F462" s="16"/>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A463" s="5" t="s">
         <v>946</v>
       </c>
@@ -29455,7 +29471,7 @@
       <c r="E463" s="5"/>
       <c r="F463" s="16"/>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A464" s="5" t="s">
         <v>947</v>
       </c>
@@ -29693,7 +29709,7 @@
       <c r="E480" s="5"/>
       <c r="F480" s="16"/>
     </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A481" s="5" t="s">
         <v>980</v>
       </c>
@@ -29707,27 +29723,30 @@
       <c r="E481" s="5"/>
       <c r="F481" s="16"/>
     </row>
-    <row r="482" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A482" s="5" t="s">
+    <row r="482" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A482" s="41" t="s">
         <v>982</v>
       </c>
-      <c r="B482" s="5" t="s">
+      <c r="B482" s="41" t="s">
         <v>983</v>
       </c>
-      <c r="C482" s="23" t="s">
+      <c r="C482" s="34" t="s">
         <v>984</v>
       </c>
-      <c r="D482" s="17" t="s">
+      <c r="D482" s="42" t="s">
         <v>982</v>
       </c>
-      <c r="E482" s="5" t="s">
+      <c r="E482" s="41" t="s">
         <v>983</v>
       </c>
-      <c r="F482" s="16" t="s">
+      <c r="F482" s="35" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G482" s="36" t="s">
+        <v>7346</v>
+      </c>
+    </row>
+    <row r="483" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A483" s="5" t="s">
         <v>985</v>
       </c>
@@ -29741,7 +29760,7 @@
       <c r="E483" s="5"/>
       <c r="F483" s="16"/>
     </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A484" s="5" t="s">
         <v>986</v>
       </c>
@@ -29755,7 +29774,7 @@
       <c r="E484" s="5"/>
       <c r="F484" s="16"/>
     </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A485" s="5" t="s">
         <v>988</v>
       </c>
@@ -29769,7 +29788,7 @@
       <c r="E485" s="5"/>
       <c r="F485" s="16"/>
     </row>
-    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A486" s="5" t="s">
         <v>990</v>
       </c>
@@ -29783,7 +29802,7 @@
       <c r="E486" s="5"/>
       <c r="F486" s="16"/>
     </row>
-    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A487" s="5" t="s">
         <v>992</v>
       </c>
@@ -29797,7 +29816,7 @@
       <c r="E487" s="5"/>
       <c r="F487" s="16"/>
     </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A488" s="5" t="s">
         <v>994</v>
       </c>
@@ -29811,7 +29830,7 @@
       <c r="E488" s="5"/>
       <c r="F488" s="16"/>
     </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A489" s="5" t="s">
         <v>996</v>
       </c>
@@ -29825,7 +29844,7 @@
       <c r="E489" s="5"/>
       <c r="F489" s="16"/>
     </row>
-    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A490" s="5" t="s">
         <v>998</v>
       </c>
@@ -29839,7 +29858,7 @@
       <c r="E490" s="5"/>
       <c r="F490" s="16"/>
     </row>
-    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A491" s="5" t="s">
         <v>1000</v>
       </c>
@@ -29853,7 +29872,7 @@
       <c r="E491" s="5"/>
       <c r="F491" s="16"/>
     </row>
-    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A492" s="5" t="s">
         <v>1002</v>
       </c>
@@ -29867,7 +29886,7 @@
       <c r="E492" s="5"/>
       <c r="F492" s="16"/>
     </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A493" s="5" t="s">
         <v>1004</v>
       </c>
@@ -29881,7 +29900,7 @@
       <c r="E493" s="5"/>
       <c r="F493" s="16"/>
     </row>
-    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A494" s="5" t="s">
         <v>1006</v>
       </c>
@@ -29895,7 +29914,7 @@
       <c r="E494" s="5"/>
       <c r="F494" s="16"/>
     </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A495" s="5" t="s">
         <v>1008</v>
       </c>
@@ -29909,7 +29928,7 @@
       <c r="E495" s="5"/>
       <c r="F495" s="16"/>
     </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A496" s="5" t="s">
         <v>1010</v>
       </c>
@@ -30369,7 +30388,7 @@
       <c r="E528" s="5"/>
       <c r="F528" s="16"/>
     </row>
-    <row r="529" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A529" s="5" t="s">
         <v>1079</v>
       </c>
@@ -30383,7 +30402,7 @@
       <c r="E529" s="5"/>
       <c r="F529" s="16"/>
     </row>
-    <row r="530" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A530" s="5" t="s">
         <v>1081</v>
       </c>
@@ -30397,7 +30416,7 @@
       <c r="E530" s="5"/>
       <c r="F530" s="16"/>
     </row>
-    <row r="531" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A531" s="5" t="s">
         <v>1083</v>
       </c>
@@ -30411,7 +30430,7 @@
       <c r="E531" s="5"/>
       <c r="F531" s="16"/>
     </row>
-    <row r="532" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A532" s="5" t="s">
         <v>1085</v>
       </c>
@@ -30425,7 +30444,7 @@
       <c r="E532" s="5"/>
       <c r="F532" s="16"/>
     </row>
-    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A533" s="5" t="s">
         <v>1087</v>
       </c>
@@ -30439,7 +30458,7 @@
       <c r="E533" s="5"/>
       <c r="F533" s="16"/>
     </row>
-    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A534" s="5" t="s">
         <v>1089</v>
       </c>
@@ -30453,7 +30472,7 @@
       <c r="E534" s="5"/>
       <c r="F534" s="16"/>
     </row>
-    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A535" s="5" t="s">
         <v>1091</v>
       </c>
@@ -30467,7 +30486,7 @@
       <c r="E535" s="5"/>
       <c r="F535" s="16"/>
     </row>
-    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A536" s="5" t="s">
         <v>1093</v>
       </c>
@@ -30481,7 +30500,7 @@
       <c r="E536" s="5"/>
       <c r="F536" s="16"/>
     </row>
-    <row r="537" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A537" s="5" t="s">
         <v>1095</v>
       </c>
@@ -30495,7 +30514,7 @@
       <c r="E537" s="5"/>
       <c r="F537" s="16"/>
     </row>
-    <row r="538" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A538" s="5" t="s">
         <v>1097</v>
       </c>
@@ -30509,7 +30528,7 @@
       <c r="E538" s="5"/>
       <c r="F538" s="16"/>
     </row>
-    <row r="539" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A539" s="5" t="s">
         <v>1099</v>
       </c>
@@ -30523,7 +30542,7 @@
       <c r="E539" s="5"/>
       <c r="F539" s="16"/>
     </row>
-    <row r="540" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A540" s="5" t="s">
         <v>1101</v>
       </c>
@@ -30537,7 +30556,7 @@
       <c r="E540" s="5"/>
       <c r="F540" s="16"/>
     </row>
-    <row r="541" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A541" s="5" t="s">
         <v>1103</v>
       </c>
@@ -30551,27 +30570,30 @@
       <c r="E541" s="5"/>
       <c r="F541" s="16"/>
     </row>
-    <row r="542" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A542" s="5" t="s">
+    <row r="542" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A542" s="41" t="s">
         <v>1105</v>
       </c>
-      <c r="B542" s="5" t="s">
+      <c r="B542" s="41" t="s">
         <v>1106</v>
       </c>
-      <c r="C542" s="23" t="s">
+      <c r="C542" s="34" t="s">
         <v>1107</v>
       </c>
-      <c r="D542" s="17" t="s">
+      <c r="D542" s="42" t="s">
         <v>1105</v>
       </c>
-      <c r="E542" s="5" t="s">
+      <c r="E542" s="41" t="s">
         <v>1106</v>
       </c>
-      <c r="F542" s="16" t="s">
+      <c r="F542" s="35" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="543" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G542" s="36" t="s">
+        <v>7347</v>
+      </c>
+    </row>
+    <row r="543" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A543" s="5" t="s">
         <v>1108</v>
       </c>
@@ -30585,7 +30607,7 @@
       <c r="E543" s="5"/>
       <c r="F543" s="16"/>
     </row>
-    <row r="544" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A544" s="5" t="s">
         <v>1110</v>
       </c>

</xml_diff>

<commit_message>
#27 reconcile: MOP:0000582, MOP:0000583,
MOP:0000584, MOP:0000585, MOP:0000586, MOP:0000587 and MOP:0000588
</commit_message>
<xml_diff>
--- a/MOP_vs_RXNO.xlsx
+++ b/MOP_vs_RXNO.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11127" uniqueCount="7360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11134" uniqueCount="7363">
   <si>
     <t>ID</t>
   </si>
@@ -22220,6 +22220,15 @@
   <si>
     <t>use MOP version</t>
   </si>
+  <si>
+    <t>use RXNO version, as this seems to be more precise</t>
+  </si>
+  <si>
+    <t>use RXNO version, as this seems to be more precise; leaves oxidated cleavage dangling</t>
+  </si>
+  <si>
+    <t>use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete.</t>
+  </si>
 </sst>
 </file>
 
@@ -22257,7 +22266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -22273,6 +22282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -22599,7 +22614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -22689,9 +22704,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -23000,8 +23023,8 @@
   <dimension ref="A1:H3631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A581" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F586" sqref="F586"/>
+      <pane ySplit="2" topLeftCell="A580" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D585" sqref="D585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31305,7 +31328,7 @@
       <c r="D576" s="27" t="s">
         <v>1183</v>
       </c>
-      <c r="E576" s="41" t="s">
+      <c r="E576" s="42" t="s">
         <v>1185</v>
       </c>
       <c r="F576" s="21" t="s">
@@ -31328,7 +31351,7 @@
       <c r="D577" s="27" t="s">
         <v>1187</v>
       </c>
-      <c r="E577" s="41" t="s">
+      <c r="E577" s="42" t="s">
         <v>1189</v>
       </c>
       <c r="F577" s="21" t="s">
@@ -31500,143 +31523,164 @@
       </c>
     </row>
     <row r="585" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A585" s="3" t="s">
+      <c r="A585" s="23" t="s">
         <v>1210</v>
       </c>
-      <c r="B585" s="32" t="s">
+      <c r="B585" s="33" t="s">
         <v>1211</v>
       </c>
-      <c r="C585" s="11" t="s">
+      <c r="C585" s="24" t="s">
         <v>1209</v>
       </c>
-      <c r="D585" s="6" t="s">
+      <c r="D585" s="25" t="s">
         <v>1210</v>
       </c>
-      <c r="E585" s="32" t="s">
+      <c r="E585" s="33" t="s">
         <v>1211</v>
       </c>
-      <c r="F585" s="11" t="s">
+      <c r="F585" s="24" t="s">
         <v>1209</v>
       </c>
+      <c r="G585" s="22" t="s">
+        <v>7359</v>
+      </c>
     </row>
     <row r="586" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A586" s="3" t="s">
+      <c r="A586" s="23" t="s">
         <v>1212</v>
       </c>
-      <c r="B586" s="32" t="s">
+      <c r="B586" s="33" t="s">
         <v>1213</v>
       </c>
-      <c r="C586" s="11" t="s">
+      <c r="C586" s="24" t="s">
         <v>1214</v>
       </c>
-      <c r="D586" s="6" t="s">
+      <c r="D586" s="25" t="s">
         <v>1212</v>
       </c>
-      <c r="E586" s="32" t="s">
+      <c r="E586" s="33" t="s">
         <v>1213</v>
       </c>
-      <c r="F586" s="11" t="s">
+      <c r="F586" s="24" t="s">
         <v>1214</v>
       </c>
+      <c r="G586" s="22" t="s">
+        <v>7359</v>
+      </c>
     </row>
     <row r="587" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A587" s="3" t="s">
+      <c r="A587" s="43" t="s">
         <v>1215</v>
       </c>
-      <c r="B587" s="32" t="s">
+      <c r="B587" s="41" t="s">
         <v>1216</v>
       </c>
-      <c r="C587" s="11" t="s">
+      <c r="C587" s="44" t="s">
         <v>1217</v>
       </c>
-      <c r="D587" s="6" t="s">
+      <c r="D587" s="45" t="s">
         <v>1215</v>
       </c>
-      <c r="E587" s="32" t="s">
+      <c r="E587" s="41" t="s">
         <v>1216</v>
       </c>
-      <c r="F587" s="11" t="s">
+      <c r="F587" s="44" t="s">
         <v>1218</v>
       </c>
+      <c r="G587" s="22" t="s">
+        <v>7361</v>
+      </c>
     </row>
     <row r="588" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A588" s="3" t="s">
+      <c r="A588" s="43" t="s">
         <v>1219</v>
       </c>
-      <c r="B588" s="32" t="s">
+      <c r="B588" s="41" t="s">
         <v>1220</v>
       </c>
-      <c r="C588" s="11" t="s">
+      <c r="C588" s="44" t="s">
         <v>1217</v>
       </c>
-      <c r="D588" s="6" t="s">
+      <c r="D588" s="45" t="s">
         <v>1219</v>
       </c>
-      <c r="E588" s="32" t="s">
+      <c r="E588" s="41" t="s">
         <v>1220</v>
       </c>
-      <c r="F588" s="11" t="s">
+      <c r="F588" s="44" t="s">
         <v>1221</v>
       </c>
+      <c r="G588" s="22" t="s">
+        <v>7360</v>
+      </c>
     </row>
     <row r="589" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A589" s="3" t="s">
+      <c r="A589" s="43" t="s">
         <v>1222</v>
       </c>
-      <c r="B589" s="32" t="s">
+      <c r="B589" s="41" t="s">
         <v>1223</v>
       </c>
-      <c r="C589" s="11" t="s">
+      <c r="C589" s="44" t="s">
         <v>1217</v>
       </c>
-      <c r="D589" s="6" t="s">
+      <c r="D589" s="45" t="s">
         <v>1222</v>
       </c>
-      <c r="E589" s="32" t="s">
+      <c r="E589" s="41" t="s">
         <v>1223</v>
       </c>
-      <c r="F589" s="11" t="s">
+      <c r="F589" s="44" t="s">
         <v>1224</v>
       </c>
+      <c r="G589" s="22" t="s">
+        <v>7360</v>
+      </c>
     </row>
     <row r="590" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A590" s="3" t="s">
+      <c r="A590" s="43" t="s">
         <v>1225</v>
       </c>
-      <c r="B590" s="32" t="s">
+      <c r="B590" s="41" t="s">
         <v>1226</v>
       </c>
-      <c r="C590" s="11" t="s">
+      <c r="C590" s="44" t="s">
         <v>1217</v>
       </c>
-      <c r="D590" s="6" t="s">
+      <c r="D590" s="45" t="s">
         <v>1225</v>
       </c>
-      <c r="E590" s="32" t="s">
+      <c r="E590" s="41" t="s">
         <v>1226</v>
       </c>
-      <c r="F590" s="11" t="s">
+      <c r="F590" s="44" t="s">
         <v>1227</v>
       </c>
+      <c r="G590" s="22" t="s">
+        <v>7360</v>
+      </c>
     </row>
     <row r="591" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A591" s="3" t="s">
+      <c r="A591" s="43" t="s">
         <v>1228</v>
       </c>
-      <c r="B591" s="32" t="s">
+      <c r="B591" s="41" t="s">
         <v>1229</v>
       </c>
-      <c r="C591" s="11" t="s">
+      <c r="C591" s="44" t="s">
         <v>1217</v>
       </c>
-      <c r="D591" s="6" t="s">
+      <c r="D591" s="45" t="s">
         <v>1228</v>
       </c>
-      <c r="E591" s="32" t="s">
+      <c r="E591" s="41" t="s">
         <v>1229</v>
       </c>
-      <c r="F591" s="11" t="s">
+      <c r="F591" s="44" t="s">
         <v>1221</v>
+      </c>
+      <c r="G591" s="22" t="s">
+        <v>7362</v>
       </c>
     </row>
     <row r="592" spans="1:7" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#27 propose how to classify 'alkene oxidative cleavage' for now
</commit_message>
<xml_diff>
--- a/MOP_vs_RXNO.xlsx
+++ b/MOP_vs_RXNO.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11134" uniqueCount="7363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11134" uniqueCount="7362">
   <si>
     <t>ID</t>
   </si>
@@ -22221,13 +22221,10 @@
     <t>use MOP version</t>
   </si>
   <si>
-    <t>use RXNO version, as this seems to be more precise</t>
-  </si>
-  <si>
-    <t>use RXNO version, as this seems to be more precise; leaves oxidated cleavage dangling</t>
-  </si>
-  <si>
     <t>use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete.</t>
+  </si>
+  <si>
+    <t>use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete. Also for now make the parent 'alkene oxidative cleavage' also a child of 'oxidative cleavage' undtil this can be inffered instead of being asserted.</t>
   </si>
 </sst>
 </file>
@@ -23023,8 +23020,8 @@
   <dimension ref="A1:H3631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A580" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D585" sqref="D585"/>
+      <pane ySplit="2" topLeftCell="A588" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G590" sqref="G590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31588,7 +31585,7 @@
         <v>1218</v>
       </c>
       <c r="G587" s="22" t="s">
-        <v>7361</v>
+        <v>7360</v>
       </c>
     </row>
     <row r="588" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -31611,7 +31608,7 @@
         <v>1221</v>
       </c>
       <c r="G588" s="22" t="s">
-        <v>7360</v>
+        <v>7361</v>
       </c>
     </row>
     <row r="589" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -31634,7 +31631,7 @@
         <v>1224</v>
       </c>
       <c r="G589" s="22" t="s">
-        <v>7360</v>
+        <v>7361</v>
       </c>
     </row>
     <row r="590" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -31657,10 +31654,10 @@
         <v>1227</v>
       </c>
       <c r="G590" s="22" t="s">
-        <v>7360</v>
-      </c>
-    </row>
-    <row r="591" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>7361</v>
+      </c>
+    </row>
+    <row r="591" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A591" s="43" t="s">
         <v>1228</v>
       </c>
@@ -31680,7 +31677,7 @@
         <v>1221</v>
       </c>
       <c r="G591" s="22" t="s">
-        <v>7362</v>
+        <v>7361</v>
       </c>
     </row>
     <row r="592" spans="1:7" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#27 reconcile: MOP:0000589, MOP:0000596, MOP:0000618, ...
MOP:0000619, MOP:0000627, MOP:0000628, MOP:0000642, MOP:0000650, MOP:0000656, MOP:0000671, MOP:0000705, MOP:0000713, MOP:0000714,  MOP:0000715,  MOP:0000716,  MOP:0000717,  MOP:0000718,  MOP:0000719,  MOP:0000720
</commit_message>
<xml_diff>
--- a/MOP_vs_RXNO.xlsx
+++ b/MOP_vs_RXNO.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11134" uniqueCount="7362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11155" uniqueCount="7371">
   <si>
     <t>ID</t>
   </si>
@@ -22203,9 +22203,6 @@
     </r>
   </si>
   <si>
-    <t>use MOP version, as ist parent is more precise</t>
-  </si>
-  <si>
     <t>copy subclassOf axioms from RXNO version to MOP</t>
   </si>
   <si>
@@ -22215,23 +22212,53 @@
     <t>copy subclassOf axioms from RXNO version to MOP; which label?</t>
   </si>
   <si>
-    <t>use RXNO version as ist parent is more precise</t>
-  </si>
-  <si>
     <t>use MOP version</t>
   </si>
   <si>
-    <t>use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete.</t>
-  </si>
-  <si>
     <t>use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete. Also for now make the parent 'alkene oxidative cleavage' also a child of 'oxidative cleavage' undtil this can be inffered instead of being asserted.</t>
+  </si>
+  <si>
+    <t>use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete. Also add axioms on 'alkene oxidative cleavage and 'oxidative cleavage'</t>
+  </si>
+  <si>
+    <t>use MOP version but keep has_alternative_id annotation</t>
+  </si>
+  <si>
+    <t>use MOP version but keep RXNO label as alternative label</t>
+  </si>
+  <si>
+    <t>use MOP Version</t>
+  </si>
+  <si>
+    <t>use RXNO version as its parent is more precise</t>
+  </si>
+  <si>
+    <t>use MOP version, as its parent is more precise</t>
+  </si>
+  <si>
+    <t>mint new ID for oxidation state and make annotation to wrong id</t>
+  </si>
+  <si>
+    <t>MOP:0000591 is the correct ID for 'carboxylation' --&gt; affects subclass RXNO:0000182, but copy has participant axiom to MOP:0000591, also make comments to reflect this change; change parent (acylation) to be a subclass of  "organylation" as it is in RXNO and not just a sibling as it is in MOP right now</t>
+  </si>
+  <si>
+    <t>"carbonyl oxidation to alkyne" has wrong ID, as this was taken by MOP already, thus needs a new ID to be minted in MOP</t>
+  </si>
+  <si>
+    <t>"[3+2] cycloaddition" has wrong ID, as this was taken by MOP already, thus needs a new ID to be minted in MOP</t>
+  </si>
+  <si>
+    <t>"enolization" is MOP:0000672 --&gt; wrong ID in RXNO; sync axioms and use MOP parent 'keto-enol tautomerisation'</t>
+  </si>
+  <si>
+    <t>cut to MOP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -22262,8 +22289,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -22285,6 +22320,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -22608,10 +22649,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -22686,6 +22728,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -22701,19 +22757,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -23020,8 +23082,8 @@
   <dimension ref="A1:H3631"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A588" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G590" sqref="G590"/>
+      <pane ySplit="2" topLeftCell="A715" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G723" sqref="G723"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23029,7 +23091,7 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="14" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" style="14" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" style="14" customWidth="1"/>
     <col min="7" max="7" width="54.85546875" style="22" customWidth="1"/>
@@ -23037,16 +23099,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>7338</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44" t="s">
         <v>7339</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="46"/>
       <c r="G1" s="19" t="s">
         <v>7340</v>
       </c>
@@ -31171,7 +31233,7 @@
         <v>1115</v>
       </c>
       <c r="G569" s="22" t="s">
-        <v>7354</v>
+        <v>7364</v>
       </c>
     </row>
     <row r="570" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -31194,7 +31256,7 @@
         <v>1115</v>
       </c>
       <c r="G570" s="22" t="s">
-        <v>7354</v>
+        <v>7364</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.25">
@@ -31286,7 +31348,7 @@
         <v>1179</v>
       </c>
       <c r="G574" s="22" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
     </row>
     <row r="575" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -31309,7 +31371,7 @@
         <v>1182</v>
       </c>
       <c r="G575" s="22" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
     </row>
     <row r="576" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -31325,14 +31387,14 @@
       <c r="D576" s="27" t="s">
         <v>1183</v>
       </c>
-      <c r="E576" s="42" t="s">
+      <c r="E576" s="37" t="s">
         <v>1185</v>
       </c>
       <c r="F576" s="21" t="s">
         <v>1186</v>
       </c>
       <c r="G576" s="22" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
     </row>
     <row r="577" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -31348,14 +31410,14 @@
       <c r="D577" s="27" t="s">
         <v>1187</v>
       </c>
-      <c r="E577" s="42" t="s">
+      <c r="E577" s="37" t="s">
         <v>1189</v>
       </c>
       <c r="F577" s="21" t="s">
         <v>1190</v>
       </c>
       <c r="G577" s="22" t="s">
-        <v>7357</v>
+        <v>7356</v>
       </c>
     </row>
     <row r="578" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -31378,7 +31440,7 @@
         <v>1193</v>
       </c>
       <c r="G578" s="22" t="s">
-        <v>7358</v>
+        <v>7363</v>
       </c>
     </row>
     <row r="579" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -31401,7 +31463,7 @@
         <v>1174</v>
       </c>
       <c r="G579" s="22" t="s">
-        <v>7359</v>
+        <v>7357</v>
       </c>
     </row>
     <row r="580" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -31424,7 +31486,7 @@
         <v>1198</v>
       </c>
       <c r="G580" s="22" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
     </row>
     <row r="581" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -31447,7 +31509,7 @@
         <v>1201</v>
       </c>
       <c r="G581" s="22" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
     </row>
     <row r="582" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -31470,7 +31532,7 @@
         <v>1204</v>
       </c>
       <c r="G582" s="22" t="s">
-        <v>7356</v>
+        <v>7355</v>
       </c>
     </row>
     <row r="583" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -31493,7 +31555,7 @@
         <v>1207</v>
       </c>
       <c r="G583" s="22" t="s">
-        <v>7355</v>
+        <v>7354</v>
       </c>
     </row>
     <row r="584" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -31516,7 +31578,7 @@
         <v>1172</v>
       </c>
       <c r="G584" s="22" t="s">
-        <v>7359</v>
+        <v>7357</v>
       </c>
     </row>
     <row r="585" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -31539,7 +31601,7 @@
         <v>1209</v>
       </c>
       <c r="G585" s="22" t="s">
-        <v>7359</v>
+        <v>7357</v>
       </c>
     </row>
     <row r="586" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -31562,145 +31624,148 @@
         <v>1214</v>
       </c>
       <c r="G586" s="22" t="s">
+        <v>7357</v>
+      </c>
+    </row>
+    <row r="587" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A587" s="38" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B587" s="36" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C587" s="39" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D587" s="40" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E587" s="36" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F587" s="39" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G587" s="41" t="s">
         <v>7359</v>
       </c>
     </row>
-    <row r="587" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A587" s="43" t="s">
-        <v>1215</v>
-      </c>
-      <c r="B587" s="41" t="s">
-        <v>1216</v>
-      </c>
-      <c r="C587" s="44" t="s">
+    <row r="588" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A588" s="38" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B588" s="36" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C588" s="39" t="s">
         <v>1217</v>
       </c>
-      <c r="D587" s="45" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E587" s="41" t="s">
-        <v>1216</v>
-      </c>
-      <c r="F587" s="44" t="s">
-        <v>1218</v>
-      </c>
-      <c r="G587" s="22" t="s">
-        <v>7360</v>
-      </c>
-    </row>
-    <row r="588" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A588" s="43" t="s">
+      <c r="D588" s="40" t="s">
         <v>1219</v>
       </c>
-      <c r="B588" s="41" t="s">
+      <c r="E588" s="36" t="s">
         <v>1220</v>
       </c>
-      <c r="C588" s="44" t="s">
+      <c r="F588" s="39" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G588" s="41" t="s">
+        <v>7359</v>
+      </c>
+    </row>
+    <row r="589" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A589" s="38" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B589" s="36" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C589" s="39" t="s">
         <v>1217</v>
       </c>
-      <c r="D588" s="45" t="s">
-        <v>1219</v>
-      </c>
-      <c r="E588" s="41" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F588" s="44" t="s">
+      <c r="D589" s="40" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E589" s="36" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F589" s="39" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G589" s="41" t="s">
+        <v>7359</v>
+      </c>
+    </row>
+    <row r="590" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A590" s="38" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B590" s="36" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C590" s="39" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D590" s="40" t="s">
+        <v>1225</v>
+      </c>
+      <c r="E590" s="36" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F590" s="39" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G590" s="22" t="s">
+        <v>7358</v>
+      </c>
+    </row>
+    <row r="591" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A591" s="38" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B591" s="36" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C591" s="39" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D591" s="40" t="s">
+        <v>1228</v>
+      </c>
+      <c r="E591" s="36" t="s">
+        <v>1229</v>
+      </c>
+      <c r="F591" s="39" t="s">
         <v>1221</v>
       </c>
-      <c r="G588" s="22" t="s">
-        <v>7361</v>
-      </c>
-    </row>
-    <row r="589" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A589" s="43" t="s">
-        <v>1222</v>
-      </c>
-      <c r="B589" s="41" t="s">
-        <v>1223</v>
-      </c>
-      <c r="C589" s="44" t="s">
-        <v>1217</v>
-      </c>
-      <c r="D589" s="45" t="s">
-        <v>1222</v>
-      </c>
-      <c r="E589" s="41" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F589" s="44" t="s">
-        <v>1224</v>
-      </c>
-      <c r="G589" s="22" t="s">
-        <v>7361</v>
-      </c>
-    </row>
-    <row r="590" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A590" s="43" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B590" s="41" t="s">
-        <v>1226</v>
-      </c>
-      <c r="C590" s="44" t="s">
-        <v>1217</v>
-      </c>
-      <c r="D590" s="45" t="s">
-        <v>1225</v>
-      </c>
-      <c r="E590" s="41" t="s">
-        <v>1226</v>
-      </c>
-      <c r="F590" s="44" t="s">
-        <v>1227</v>
-      </c>
-      <c r="G590" s="22" t="s">
-        <v>7361</v>
-      </c>
-    </row>
-    <row r="591" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A591" s="43" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B591" s="41" t="s">
-        <v>1229</v>
-      </c>
-      <c r="C591" s="44" t="s">
-        <v>1217</v>
-      </c>
-      <c r="D591" s="45" t="s">
-        <v>1228</v>
-      </c>
-      <c r="E591" s="41" t="s">
-        <v>1229</v>
-      </c>
-      <c r="F591" s="44" t="s">
-        <v>1221</v>
-      </c>
-      <c r="G591" s="22" t="s">
-        <v>7361</v>
+      <c r="G591" s="41" t="s">
+        <v>7359</v>
       </c>
     </row>
     <row r="592" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A592" s="3" t="s">
+      <c r="A592" s="23" t="s">
         <v>1230</v>
       </c>
-      <c r="B592" s="32" t="s">
+      <c r="B592" s="33" t="s">
         <v>1231</v>
       </c>
-      <c r="C592" s="11" t="s">
+      <c r="C592" s="24" t="s">
         <v>1174</v>
       </c>
-      <c r="D592" s="6" t="s">
+      <c r="D592" s="25" t="s">
         <v>1230</v>
       </c>
-      <c r="E592" s="32" t="s">
+      <c r="E592" s="33" t="s">
         <v>1231</v>
       </c>
-      <c r="F592" s="11" t="s">
+      <c r="F592" s="24" t="s">
         <v>1174</v>
       </c>
-    </row>
-    <row r="593" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G592" s="22" t="s">
+        <v>7357</v>
+      </c>
+    </row>
+    <row r="593" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A593" s="3" t="s">
         <v>1232</v>
       </c>
@@ -31714,7 +31779,7 @@
       <c r="E593" s="32"/>
       <c r="F593" s="11"/>
     </row>
-    <row r="594" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A594" s="3" t="s">
         <v>1234</v>
       </c>
@@ -31728,7 +31793,7 @@
       <c r="E594" s="32"/>
       <c r="F594" s="11"/>
     </row>
-    <row r="595" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A595" s="3" t="s">
         <v>1236</v>
       </c>
@@ -31742,7 +31807,7 @@
       <c r="E595" s="32"/>
       <c r="F595" s="11"/>
     </row>
-    <row r="596" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A596" s="3" t="s">
         <v>1238</v>
       </c>
@@ -31756,7 +31821,7 @@
       <c r="E596" s="32"/>
       <c r="F596" s="11"/>
     </row>
-    <row r="597" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A597" s="3" t="s">
         <v>1240</v>
       </c>
@@ -31770,7 +31835,7 @@
       <c r="E597" s="32"/>
       <c r="F597" s="11"/>
     </row>
-    <row r="598" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A598" s="3" t="s">
         <v>1242</v>
       </c>
@@ -31784,27 +31849,30 @@
       <c r="E598" s="32"/>
       <c r="F598" s="11"/>
     </row>
-    <row r="599" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A599" s="3" t="s">
+    <row r="599" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A599" s="23" t="s">
         <v>1244</v>
       </c>
-      <c r="B599" s="32" t="s">
+      <c r="B599" s="33" t="s">
         <v>1245</v>
       </c>
-      <c r="C599" s="11" t="s">
+      <c r="C599" s="24" t="s">
         <v>1246</v>
       </c>
-      <c r="D599" s="6" t="s">
+      <c r="D599" s="25" t="s">
         <v>1244</v>
       </c>
-      <c r="E599" s="32" t="s">
+      <c r="E599" s="33" t="s">
         <v>1245</v>
       </c>
-      <c r="F599" s="11" t="s">
+      <c r="F599" s="24" t="s">
         <v>1247</v>
       </c>
-    </row>
-    <row r="600" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G599" s="22" t="s">
+        <v>7357</v>
+      </c>
+    </row>
+    <row r="600" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A600" s="3" t="s">
         <v>1248</v>
       </c>
@@ -31818,7 +31886,7 @@
       <c r="E600" s="32"/>
       <c r="F600" s="11"/>
     </row>
-    <row r="601" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A601" s="3" t="s">
         <v>1251</v>
       </c>
@@ -31832,7 +31900,7 @@
       <c r="E601" s="32"/>
       <c r="F601" s="11"/>
     </row>
-    <row r="602" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A602" s="3" t="s">
         <v>1254</v>
       </c>
@@ -31846,7 +31914,7 @@
       <c r="E602" s="32"/>
       <c r="F602" s="11"/>
     </row>
-    <row r="603" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A603" s="3" t="s">
         <v>1257</v>
       </c>
@@ -31860,7 +31928,7 @@
       <c r="E603" s="32"/>
       <c r="F603" s="11"/>
     </row>
-    <row r="604" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A604" s="3" t="s">
         <v>1260</v>
       </c>
@@ -31874,7 +31942,7 @@
       <c r="E604" s="32"/>
       <c r="F604" s="11"/>
     </row>
-    <row r="605" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A605" s="3" t="s">
         <v>1263</v>
       </c>
@@ -31888,7 +31956,7 @@
       <c r="E605" s="32"/>
       <c r="F605" s="11"/>
     </row>
-    <row r="606" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A606" s="3" t="s">
         <v>1266</v>
       </c>
@@ -31902,7 +31970,7 @@
       <c r="E606" s="32"/>
       <c r="F606" s="11"/>
     </row>
-    <row r="607" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A607" s="3" t="s">
         <v>1269</v>
       </c>
@@ -31916,7 +31984,7 @@
       <c r="E607" s="32"/>
       <c r="F607" s="11"/>
     </row>
-    <row r="608" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A608" s="3" t="s">
         <v>1272</v>
       </c>
@@ -31930,7 +31998,7 @@
       <c r="E608" s="32"/>
       <c r="F608" s="11"/>
     </row>
-    <row r="609" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A609" s="3" t="s">
         <v>1274</v>
       </c>
@@ -31944,7 +32012,7 @@
       <c r="E609" s="32"/>
       <c r="F609" s="11"/>
     </row>
-    <row r="610" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A610" s="3" t="s">
         <v>1276</v>
       </c>
@@ -31958,7 +32026,7 @@
       <c r="E610" s="32"/>
       <c r="F610" s="11"/>
     </row>
-    <row r="611" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A611" s="3" t="s">
         <v>1278</v>
       </c>
@@ -31972,7 +32040,7 @@
       <c r="E611" s="32"/>
       <c r="F611" s="11"/>
     </row>
-    <row r="612" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A612" s="3" t="s">
         <v>1280</v>
       </c>
@@ -31986,7 +32054,7 @@
       <c r="E612" s="32"/>
       <c r="F612" s="11"/>
     </row>
-    <row r="613" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A613" s="3" t="s">
         <v>1282</v>
       </c>
@@ -32000,7 +32068,7 @@
       <c r="E613" s="32"/>
       <c r="F613" s="11"/>
     </row>
-    <row r="614" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A614" s="3" t="s">
         <v>1284</v>
       </c>
@@ -32014,7 +32082,7 @@
       <c r="E614" s="32"/>
       <c r="F614" s="11"/>
     </row>
-    <row r="615" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A615" s="3" t="s">
         <v>1286</v>
       </c>
@@ -32028,7 +32096,7 @@
       <c r="E615" s="32"/>
       <c r="F615" s="11"/>
     </row>
-    <row r="616" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A616" s="3" t="s">
         <v>1288</v>
       </c>
@@ -32042,7 +32110,7 @@
       <c r="E616" s="32"/>
       <c r="F616" s="11"/>
     </row>
-    <row r="617" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A617" s="3" t="s">
         <v>1290</v>
       </c>
@@ -32056,7 +32124,7 @@
       <c r="E617" s="32"/>
       <c r="F617" s="11"/>
     </row>
-    <row r="618" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A618" s="3" t="s">
         <v>1292</v>
       </c>
@@ -32070,7 +32138,7 @@
       <c r="E618" s="32"/>
       <c r="F618" s="11"/>
     </row>
-    <row r="619" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A619" s="3" t="s">
         <v>1294</v>
       </c>
@@ -32084,7 +32152,7 @@
       <c r="E619" s="32"/>
       <c r="F619" s="11"/>
     </row>
-    <row r="620" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A620" s="3" t="s">
         <v>1296</v>
       </c>
@@ -32098,47 +32166,53 @@
       <c r="E620" s="32"/>
       <c r="F620" s="11"/>
     </row>
-    <row r="621" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A621" s="3" t="s">
+    <row r="621" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A621" s="47" t="s">
         <v>1298</v>
       </c>
-      <c r="B621" s="32" t="s">
+      <c r="B621" s="48" t="s">
         <v>1299</v>
       </c>
-      <c r="C621" s="11" t="s">
+      <c r="C621" s="49" t="s">
         <v>1115</v>
       </c>
-      <c r="D621" s="6" t="s">
+      <c r="D621" s="50" t="s">
         <v>1298</v>
       </c>
-      <c r="E621" s="32" t="s">
+      <c r="E621" s="48" t="s">
         <v>1299</v>
       </c>
-      <c r="F621" s="11" t="s">
+      <c r="F621" s="49" t="s">
         <v>1115</v>
       </c>
-    </row>
-    <row r="622" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A622" s="3" t="s">
+      <c r="G621" s="22" t="s">
+        <v>7357</v>
+      </c>
+    </row>
+    <row r="622" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A622" s="23" t="s">
         <v>1300</v>
       </c>
-      <c r="B622" s="32" t="s">
+      <c r="B622" s="33" t="s">
         <v>1301</v>
       </c>
-      <c r="C622" s="11" t="s">
+      <c r="C622" s="24" t="s">
         <v>1299</v>
       </c>
-      <c r="D622" s="6" t="s">
+      <c r="D622" s="25" t="s">
         <v>1300</v>
       </c>
-      <c r="E622" s="32" t="s">
+      <c r="E622" s="33" t="s">
         <v>1301</v>
       </c>
-      <c r="F622" s="11" t="s">
+      <c r="F622" s="24" t="s">
         <v>1299</v>
       </c>
-    </row>
-    <row r="623" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G622" s="22" t="s">
+        <v>7357</v>
+      </c>
+    </row>
+    <row r="623" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A623" s="3" t="s">
         <v>1302</v>
       </c>
@@ -32152,7 +32226,7 @@
       <c r="E623" s="32"/>
       <c r="F623" s="11"/>
     </row>
-    <row r="624" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A624" s="3" t="s">
         <v>1304</v>
       </c>
@@ -32166,7 +32240,7 @@
       <c r="E624" s="32"/>
       <c r="F624" s="11"/>
     </row>
-    <row r="625" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A625" s="3" t="s">
         <v>1306</v>
       </c>
@@ -32180,7 +32254,7 @@
       <c r="E625" s="32"/>
       <c r="F625" s="11"/>
     </row>
-    <row r="626" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A626" s="3" t="s">
         <v>1308</v>
       </c>
@@ -32194,7 +32268,7 @@
       <c r="E626" s="32"/>
       <c r="F626" s="11"/>
     </row>
-    <row r="627" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A627" s="3" t="s">
         <v>1310</v>
       </c>
@@ -32208,7 +32282,7 @@
       <c r="E627" s="32"/>
       <c r="F627" s="11"/>
     </row>
-    <row r="628" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A628" s="3" t="s">
         <v>1312</v>
       </c>
@@ -32222,7 +32296,7 @@
       <c r="E628" s="32"/>
       <c r="F628" s="11"/>
     </row>
-    <row r="629" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A629" s="3" t="s">
         <v>1314</v>
       </c>
@@ -32236,47 +32310,53 @@
       <c r="E629" s="32"/>
       <c r="F629" s="11"/>
     </row>
-    <row r="630" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A630" s="3" t="s">
+    <row r="630" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A630" s="26" t="s">
         <v>1316</v>
       </c>
-      <c r="B630" s="32" t="s">
+      <c r="B630" s="34" t="s">
         <v>1317</v>
       </c>
-      <c r="C630" s="11" t="s">
+      <c r="C630" s="21" t="s">
         <v>1115</v>
       </c>
-      <c r="D630" s="6" t="s">
+      <c r="D630" s="27" t="s">
         <v>1316</v>
       </c>
-      <c r="E630" s="32" t="s">
+      <c r="E630" s="34" t="s">
         <v>1317</v>
       </c>
-      <c r="F630" s="11" t="s">
+      <c r="F630" s="21" t="s">
         <v>1115</v>
       </c>
-    </row>
-    <row r="631" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A631" s="3" t="s">
+      <c r="G630" s="22" t="s">
+        <v>7360</v>
+      </c>
+    </row>
+    <row r="631" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A631" s="26" t="s">
         <v>1318</v>
       </c>
-      <c r="B631" s="32" t="s">
+      <c r="B631" s="34" t="s">
         <v>1319</v>
       </c>
-      <c r="C631" s="11" t="s">
+      <c r="C631" s="21" t="s">
         <v>1317</v>
       </c>
-      <c r="D631" s="6" t="s">
+      <c r="D631" s="27" t="s">
         <v>1318</v>
       </c>
-      <c r="E631" s="32" t="s">
+      <c r="E631" s="34" t="s">
         <v>1320</v>
       </c>
-      <c r="F631" s="11" t="s">
+      <c r="F631" s="21" t="s">
         <v>1317</v>
       </c>
-    </row>
-    <row r="632" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G631" s="22" t="s">
+        <v>7361</v>
+      </c>
+    </row>
+    <row r="632" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A632" s="3" t="s">
         <v>1321</v>
       </c>
@@ -32290,7 +32370,7 @@
       <c r="E632" s="32"/>
       <c r="F632" s="11"/>
     </row>
-    <row r="633" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="633" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A633" s="3" t="s">
         <v>1324</v>
       </c>
@@ -32304,7 +32384,7 @@
       <c r="E633" s="32"/>
       <c r="F633" s="11"/>
     </row>
-    <row r="634" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="634" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A634" s="3" t="s">
         <v>1326</v>
       </c>
@@ -32318,7 +32398,7 @@
       <c r="E634" s="32"/>
       <c r="F634" s="11"/>
     </row>
-    <row r="635" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="635" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A635" s="3" t="s">
         <v>1329</v>
       </c>
@@ -32332,7 +32412,7 @@
       <c r="E635" s="32"/>
       <c r="F635" s="11"/>
     </row>
-    <row r="636" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A636" s="3" t="s">
         <v>1332</v>
       </c>
@@ -32346,7 +32426,7 @@
       <c r="E636" s="32"/>
       <c r="F636" s="11"/>
     </row>
-    <row r="637" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A637" s="3" t="s">
         <v>1335</v>
       </c>
@@ -32360,7 +32440,7 @@
       <c r="E637" s="32"/>
       <c r="F637" s="11"/>
     </row>
-    <row r="638" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="638" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A638" s="3" t="s">
         <v>1338</v>
       </c>
@@ -32374,7 +32454,7 @@
       <c r="E638" s="32"/>
       <c r="F638" s="11"/>
     </row>
-    <row r="639" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A639" s="3" t="s">
         <v>1340</v>
       </c>
@@ -32388,7 +32468,7 @@
       <c r="E639" s="32"/>
       <c r="F639" s="11"/>
     </row>
-    <row r="640" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="640" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A640" s="3" t="s">
         <v>1343</v>
       </c>
@@ -32402,7 +32482,7 @@
       <c r="E640" s="32"/>
       <c r="F640" s="11"/>
     </row>
-    <row r="641" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A641" s="3" t="s">
         <v>1344</v>
       </c>
@@ -32416,7 +32496,7 @@
       <c r="E641" s="32"/>
       <c r="F641" s="11"/>
     </row>
-    <row r="642" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A642" s="3" t="s">
         <v>1346</v>
       </c>
@@ -32430,7 +32510,7 @@
       <c r="E642" s="32"/>
       <c r="F642" s="11"/>
     </row>
-    <row r="643" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A643" s="3" t="s">
         <v>1348</v>
       </c>
@@ -32444,7 +32524,7 @@
       <c r="E643" s="32"/>
       <c r="F643" s="11"/>
     </row>
-    <row r="644" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A644" s="3" t="s">
         <v>1351</v>
       </c>
@@ -32458,27 +32538,30 @@
       <c r="E644" s="32"/>
       <c r="F644" s="11"/>
     </row>
-    <row r="645" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A645" s="3" t="s">
+    <row r="645" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A645" s="23" t="s">
         <v>1353</v>
       </c>
-      <c r="B645" s="32" t="s">
+      <c r="B645" s="33" t="s">
         <v>1354</v>
       </c>
-      <c r="C645" s="11" t="s">
+      <c r="C645" s="24" t="s">
         <v>1115</v>
       </c>
-      <c r="D645" s="6" t="s">
+      <c r="D645" s="25" t="s">
         <v>1353</v>
       </c>
-      <c r="E645" s="32" t="s">
+      <c r="E645" s="33" t="s">
         <v>1354</v>
       </c>
-      <c r="F645" s="11" t="s">
+      <c r="F645" s="24" t="s">
         <v>1115</v>
       </c>
-    </row>
-    <row r="646" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G645" s="22" t="s">
+        <v>7357</v>
+      </c>
+    </row>
+    <row r="646" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A646" s="3" t="s">
         <v>1355</v>
       </c>
@@ -32492,7 +32575,7 @@
       <c r="E646" s="32"/>
       <c r="F646" s="11"/>
     </row>
-    <row r="647" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A647" s="3" t="s">
         <v>1358</v>
       </c>
@@ -32506,7 +32589,7 @@
       <c r="E647" s="32"/>
       <c r="F647" s="11"/>
     </row>
-    <row r="648" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A648" s="3" t="s">
         <v>1361</v>
       </c>
@@ -32520,7 +32603,7 @@
       <c r="E648" s="32"/>
       <c r="F648" s="11"/>
     </row>
-    <row r="649" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A649" s="3" t="s">
         <v>1364</v>
       </c>
@@ -32534,7 +32617,7 @@
       <c r="E649" s="32"/>
       <c r="F649" s="11"/>
     </row>
-    <row r="650" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A650" s="3" t="s">
         <v>1366</v>
       </c>
@@ -32548,7 +32631,7 @@
       <c r="E650" s="32"/>
       <c r="F650" s="11"/>
     </row>
-    <row r="651" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A651" s="3" t="s">
         <v>1369</v>
       </c>
@@ -32562,7 +32645,7 @@
       <c r="E651" s="32"/>
       <c r="F651" s="11"/>
     </row>
-    <row r="652" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A652" s="3" t="s">
         <v>1372</v>
       </c>
@@ -32576,27 +32659,30 @@
       <c r="E652" s="32"/>
       <c r="F652" s="11"/>
     </row>
-    <row r="653" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A653" s="3" t="s">
+    <row r="653" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A653" s="23" t="s">
         <v>1375</v>
       </c>
-      <c r="B653" s="32" t="s">
+      <c r="B653" s="33" t="s">
         <v>1376</v>
       </c>
-      <c r="C653" s="11" t="s">
+      <c r="C653" s="24" t="s">
         <v>1377</v>
       </c>
-      <c r="D653" s="6" t="s">
+      <c r="D653" s="25" t="s">
         <v>1375</v>
       </c>
-      <c r="E653" s="32" t="s">
+      <c r="E653" s="33" t="s">
         <v>1376</v>
       </c>
-      <c r="F653" s="11" t="s">
+      <c r="F653" s="24" t="s">
         <v>1377</v>
       </c>
-    </row>
-    <row r="654" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G653" s="22" t="s">
+        <v>7362</v>
+      </c>
+    </row>
+    <row r="654" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A654" s="3" t="s">
         <v>1378</v>
       </c>
@@ -32610,7 +32696,7 @@
       <c r="E654" s="32"/>
       <c r="F654" s="11"/>
     </row>
-    <row r="655" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A655" s="3" t="s">
         <v>1381</v>
       </c>
@@ -32624,7 +32710,7 @@
       <c r="E655" s="32"/>
       <c r="F655" s="11"/>
     </row>
-    <row r="656" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A656" s="3" t="s">
         <v>1383</v>
       </c>
@@ -32638,7 +32724,7 @@
       <c r="E656" s="32"/>
       <c r="F656" s="11"/>
     </row>
-    <row r="657" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A657" s="3" t="s">
         <v>1385</v>
       </c>
@@ -32652,7 +32738,7 @@
       <c r="E657" s="32"/>
       <c r="F657" s="11"/>
     </row>
-    <row r="658" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658" s="3" t="s">
         <v>1387</v>
       </c>
@@ -32666,27 +32752,30 @@
       <c r="E658" s="32"/>
       <c r="F658" s="11"/>
     </row>
-    <row r="659" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A659" s="3" t="s">
+    <row r="659" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A659" s="23" t="s">
         <v>1389</v>
       </c>
-      <c r="B659" s="32" t="s">
+      <c r="B659" s="33" t="s">
         <v>1390</v>
       </c>
-      <c r="C659" s="11" t="s">
+      <c r="C659" s="24" t="s">
         <v>1115</v>
       </c>
-      <c r="D659" s="6" t="s">
+      <c r="D659" s="25" t="s">
         <v>1389</v>
       </c>
-      <c r="E659" s="32" t="s">
+      <c r="E659" s="33" t="s">
         <v>1390</v>
       </c>
-      <c r="F659" s="11" t="s">
+      <c r="F659" s="24" t="s">
         <v>1115</v>
       </c>
-    </row>
-    <row r="660" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G659" s="22" t="s">
+        <v>7362</v>
+      </c>
+    </row>
+    <row r="660" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A660" s="3" t="s">
         <v>1391</v>
       </c>
@@ -32700,7 +32789,7 @@
       <c r="E660" s="32"/>
       <c r="F660" s="11"/>
     </row>
-    <row r="661" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A661" s="3" t="s">
         <v>1393</v>
       </c>
@@ -32714,7 +32803,7 @@
       <c r="E661" s="32"/>
       <c r="F661" s="11"/>
     </row>
-    <row r="662" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A662" s="3" t="s">
         <v>1395</v>
       </c>
@@ -32728,7 +32817,7 @@
       <c r="E662" s="32"/>
       <c r="F662" s="11"/>
     </row>
-    <row r="663" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A663" s="3" t="s">
         <v>1397</v>
       </c>
@@ -32742,7 +32831,7 @@
       <c r="E663" s="32"/>
       <c r="F663" s="11"/>
     </row>
-    <row r="664" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A664" s="3" t="s">
         <v>1399</v>
       </c>
@@ -32756,7 +32845,7 @@
       <c r="E664" s="32"/>
       <c r="F664" s="11"/>
     </row>
-    <row r="665" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A665" s="3" t="s">
         <v>1401</v>
       </c>
@@ -32770,7 +32859,7 @@
       <c r="E665" s="32"/>
       <c r="F665" s="11"/>
     </row>
-    <row r="666" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A666" s="3" t="s">
         <v>1403</v>
       </c>
@@ -32784,7 +32873,7 @@
       <c r="E666" s="32"/>
       <c r="F666" s="11"/>
     </row>
-    <row r="667" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A667" s="3" t="s">
         <v>1405</v>
       </c>
@@ -32798,7 +32887,7 @@
       <c r="E667" s="32"/>
       <c r="F667" s="11"/>
     </row>
-    <row r="668" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A668" s="3" t="s">
         <v>1407</v>
       </c>
@@ -32812,7 +32901,7 @@
       <c r="E668" s="32"/>
       <c r="F668" s="11"/>
     </row>
-    <row r="669" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669" s="3" t="s">
         <v>1409</v>
       </c>
@@ -32826,7 +32915,7 @@
       <c r="E669" s="32"/>
       <c r="F669" s="11"/>
     </row>
-    <row r="670" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A670" s="3" t="s">
         <v>1411</v>
       </c>
@@ -32840,7 +32929,7 @@
       <c r="E670" s="32"/>
       <c r="F670" s="11"/>
     </row>
-    <row r="671" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A671" s="3" t="s">
         <v>1413</v>
       </c>
@@ -32854,7 +32943,7 @@
       <c r="E671" s="32"/>
       <c r="F671" s="11"/>
     </row>
-    <row r="672" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672" s="3" t="s">
         <v>1415</v>
       </c>
@@ -32868,7 +32957,7 @@
       <c r="E672" s="32"/>
       <c r="F672" s="11"/>
     </row>
-    <row r="673" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A673" s="3" t="s">
         <v>1417</v>
       </c>
@@ -32882,27 +32971,30 @@
       <c r="E673" s="32"/>
       <c r="F673" s="11"/>
     </row>
-    <row r="674" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A674" s="3" t="s">
+    <row r="674" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A674" s="26" t="s">
         <v>1419</v>
       </c>
-      <c r="B674" s="32" t="s">
+      <c r="B674" s="34" t="s">
         <v>1420</v>
       </c>
-      <c r="C674" s="11" t="s">
+      <c r="C674" s="21" t="s">
         <v>1421</v>
       </c>
-      <c r="D674" s="6" t="s">
+      <c r="D674" s="27" t="s">
         <v>1419</v>
       </c>
-      <c r="E674" s="32" t="s">
+      <c r="E674" s="34" t="s">
         <v>1420</v>
       </c>
-      <c r="F674" s="11" t="s">
+      <c r="F674" s="21" t="s">
         <v>1422</v>
       </c>
-    </row>
-    <row r="675" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G674" s="22" t="s">
+        <v>7363</v>
+      </c>
+    </row>
+    <row r="675" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A675" s="3" t="s">
         <v>1423</v>
       </c>
@@ -32916,7 +33008,7 @@
       <c r="E675" s="32"/>
       <c r="F675" s="11"/>
     </row>
-    <row r="676" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A676" s="3" t="s">
         <v>1426</v>
       </c>
@@ -32930,7 +33022,7 @@
       <c r="E676" s="32"/>
       <c r="F676" s="11"/>
     </row>
-    <row r="677" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" s="3" t="s">
         <v>1429</v>
       </c>
@@ -32944,7 +33036,7 @@
       <c r="E677" s="32"/>
       <c r="F677" s="11"/>
     </row>
-    <row r="678" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678" s="3" t="s">
         <v>1431</v>
       </c>
@@ -32958,7 +33050,7 @@
       <c r="E678" s="32"/>
       <c r="F678" s="11"/>
     </row>
-    <row r="679" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A679" s="3" t="s">
         <v>1434</v>
       </c>
@@ -32972,7 +33064,7 @@
       <c r="E679" s="32"/>
       <c r="F679" s="11"/>
     </row>
-    <row r="680" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A680" s="3" t="s">
         <v>1436</v>
       </c>
@@ -32986,7 +33078,7 @@
       <c r="E680" s="32"/>
       <c r="F680" s="11"/>
     </row>
-    <row r="681" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A681" s="3" t="s">
         <v>1439</v>
       </c>
@@ -33000,7 +33092,7 @@
       <c r="E681" s="32"/>
       <c r="F681" s="11"/>
     </row>
-    <row r="682" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="682" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A682" s="3" t="s">
         <v>1442</v>
       </c>
@@ -33014,7 +33106,7 @@
       <c r="E682" s="32"/>
       <c r="F682" s="11"/>
     </row>
-    <row r="683" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A683" s="3" t="s">
         <v>1445</v>
       </c>
@@ -33028,7 +33120,7 @@
       <c r="E683" s="32"/>
       <c r="F683" s="11"/>
     </row>
-    <row r="684" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="684" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A684" s="3" t="s">
         <v>1448</v>
       </c>
@@ -33042,7 +33134,7 @@
       <c r="E684" s="32"/>
       <c r="F684" s="11"/>
     </row>
-    <row r="685" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A685" s="3" t="s">
         <v>1450</v>
       </c>
@@ -33056,7 +33148,7 @@
       <c r="E685" s="32"/>
       <c r="F685" s="11"/>
     </row>
-    <row r="686" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A686" s="3" t="s">
         <v>1453</v>
       </c>
@@ -33070,7 +33162,7 @@
       <c r="E686" s="32"/>
       <c r="F686" s="11"/>
     </row>
-    <row r="687" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A687" s="3" t="s">
         <v>1456</v>
       </c>
@@ -33084,7 +33176,7 @@
       <c r="E687" s="32"/>
       <c r="F687" s="11"/>
     </row>
-    <row r="688" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A688" s="3" t="s">
         <v>1458</v>
       </c>
@@ -33322,7 +33414,7 @@
       <c r="E704" s="32"/>
       <c r="F704" s="11"/>
     </row>
-    <row r="705" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A705" s="3" t="s">
         <v>1503</v>
       </c>
@@ -33336,7 +33428,7 @@
       <c r="E705" s="32"/>
       <c r="F705" s="11"/>
     </row>
-    <row r="706" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A706" s="3" t="s">
         <v>1506</v>
       </c>
@@ -33350,7 +33442,7 @@
       <c r="E706" s="32"/>
       <c r="F706" s="11"/>
     </row>
-    <row r="707" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="707" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A707" s="3" t="s">
         <v>1509</v>
       </c>
@@ -33364,47 +33456,53 @@
       <c r="E707" s="32"/>
       <c r="F707" s="11"/>
     </row>
-    <row r="708" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A708" s="3" t="s">
+    <row r="708" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A708" s="23" t="s">
         <v>1511</v>
       </c>
-      <c r="B708" s="32" t="s">
+      <c r="B708" s="33" t="s">
         <v>1512</v>
       </c>
-      <c r="C708" s="11" t="s">
+      <c r="C708" s="24" t="s">
         <v>1172</v>
       </c>
-      <c r="D708" s="6" t="s">
+      <c r="D708" s="25" t="s">
         <v>1511</v>
       </c>
-      <c r="E708" s="32" t="s">
+      <c r="E708" s="33" t="s">
         <v>1512</v>
       </c>
-      <c r="F708" s="11" t="s">
+      <c r="F708" s="24" t="s">
         <v>1172</v>
       </c>
-    </row>
-    <row r="709" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A709" s="3" t="s">
+      <c r="G708" s="22" t="s">
+        <v>7357</v>
+      </c>
+    </row>
+    <row r="709" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A709" s="23" t="s">
         <v>1513</v>
       </c>
-      <c r="B709" s="32" t="s">
+      <c r="B709" s="33" t="s">
         <v>1193</v>
       </c>
-      <c r="C709" s="11" t="s">
+      <c r="C709" s="24" t="s">
         <v>1172</v>
       </c>
-      <c r="D709" s="6" t="s">
+      <c r="D709" s="25" t="s">
         <v>1513</v>
       </c>
-      <c r="E709" s="32" t="s">
+      <c r="E709" s="33" t="s">
         <v>1193</v>
       </c>
-      <c r="F709" s="11" t="s">
+      <c r="F709" s="24" t="s">
         <v>1172</v>
       </c>
-    </row>
-    <row r="710" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G709" s="22" t="s">
+        <v>7357</v>
+      </c>
+    </row>
+    <row r="710" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A710" s="3" t="s">
         <v>1514</v>
       </c>
@@ -33418,7 +33516,7 @@
       <c r="E710" s="32"/>
       <c r="F710" s="11"/>
     </row>
-    <row r="711" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A711" s="3" t="s">
         <v>1516</v>
       </c>
@@ -33432,7 +33530,7 @@
       <c r="E711" s="32"/>
       <c r="F711" s="11"/>
     </row>
-    <row r="712" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="712" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A712" s="3" t="s">
         <v>1517</v>
       </c>
@@ -33446,7 +33544,7 @@
       <c r="E712" s="32"/>
       <c r="F712" s="11"/>
     </row>
-    <row r="713" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="713" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A713" s="3" t="s">
         <v>1519</v>
       </c>
@@ -33460,7 +33558,7 @@
       <c r="E713" s="32"/>
       <c r="F713" s="11"/>
     </row>
-    <row r="714" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A714" s="3" t="s">
         <v>1521</v>
       </c>
@@ -33474,163 +33572,190 @@
       <c r="E714" s="32"/>
       <c r="F714" s="11"/>
     </row>
-    <row r="715" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A715" s="3" t="s">
+    <row r="715" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A715" s="51" t="s">
         <v>1524</v>
       </c>
-      <c r="B715" s="32" t="s">
+      <c r="B715" s="52" t="s">
         <v>1525</v>
       </c>
-      <c r="C715" s="11" t="s">
+      <c r="C715" s="53" t="s">
         <v>1526</v>
       </c>
-      <c r="D715" s="6" t="s">
+      <c r="D715" s="54" t="s">
         <v>1524</v>
       </c>
-      <c r="E715" s="32" t="s">
+      <c r="E715" s="52" t="s">
         <v>1527</v>
       </c>
-      <c r="F715" s="11" t="s">
+      <c r="F715" s="53" t="s">
         <v>1528</v>
       </c>
-    </row>
-    <row r="716" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A716" s="3" t="s">
+      <c r="G715" s="22" t="s">
+        <v>7365</v>
+      </c>
+    </row>
+    <row r="716" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A716" s="51" t="s">
         <v>1529</v>
       </c>
-      <c r="B716" s="32" t="s">
+      <c r="B716" s="52" t="s">
         <v>1530</v>
       </c>
-      <c r="C716" s="11" t="s">
+      <c r="C716" s="53" t="s">
         <v>1231</v>
       </c>
-      <c r="D716" s="6" t="s">
+      <c r="D716" s="54" t="s">
         <v>1529</v>
       </c>
-      <c r="E716" s="32" t="s">
+      <c r="E716" s="52" t="s">
         <v>1235</v>
       </c>
-      <c r="F716" s="11" t="s">
+      <c r="F716" s="53" t="s">
         <v>1531</v>
       </c>
-    </row>
-    <row r="717" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A717" s="3" t="s">
+      <c r="G716" s="22" t="s">
+        <v>7366</v>
+      </c>
+    </row>
+    <row r="717" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A717" s="51" t="s">
         <v>1532</v>
       </c>
-      <c r="B717" s="32" t="s">
+      <c r="B717" s="52" t="s">
         <v>1533</v>
       </c>
-      <c r="C717" s="11" t="s">
+      <c r="C717" s="53" t="s">
         <v>1534</v>
       </c>
-      <c r="D717" s="6" t="s">
+      <c r="D717" s="54" t="s">
         <v>1532</v>
       </c>
-      <c r="E717" s="32" t="s">
+      <c r="E717" s="52" t="s">
         <v>1535</v>
       </c>
-      <c r="F717" s="11" t="s">
+      <c r="F717" s="53" t="s">
         <v>1172</v>
       </c>
-    </row>
-    <row r="718" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A718" s="3" t="s">
+      <c r="G717" s="22" t="s">
+        <v>7367</v>
+      </c>
+    </row>
+    <row r="718" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A718" s="51" t="s">
         <v>1536</v>
       </c>
-      <c r="B718" s="32" t="s">
+      <c r="B718" s="52" t="s">
         <v>1537</v>
       </c>
-      <c r="C718" s="11" t="s">
+      <c r="C718" s="53" t="s">
         <v>1115</v>
       </c>
-      <c r="D718" s="6" t="s">
+      <c r="D718" s="54" t="s">
         <v>1536</v>
       </c>
-      <c r="E718" s="32" t="s">
+      <c r="E718" s="52" t="s">
         <v>1538</v>
       </c>
-      <c r="F718" s="11" t="s">
+      <c r="F718" s="53" t="s">
         <v>1158</v>
       </c>
-    </row>
-    <row r="719" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A719" s="3" t="s">
+      <c r="G718" s="22" t="s">
+        <v>7368</v>
+      </c>
+    </row>
+    <row r="719" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A719" s="51" t="s">
         <v>1539</v>
       </c>
-      <c r="B719" s="32" t="s">
+      <c r="B719" s="52" t="s">
         <v>1540</v>
       </c>
-      <c r="C719" s="11" t="s">
+      <c r="C719" s="53" t="s">
         <v>1541</v>
       </c>
-      <c r="D719" s="6" t="s">
+      <c r="D719" s="54" t="s">
         <v>1539</v>
       </c>
-      <c r="E719" s="32" t="s">
+      <c r="E719" s="52" t="s">
         <v>1542</v>
       </c>
-      <c r="F719" s="11" t="s">
+      <c r="F719" s="53" t="s">
         <v>1543</v>
       </c>
-    </row>
-    <row r="720" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G719" s="22" t="s">
+        <v>7369</v>
+      </c>
+    </row>
+    <row r="720" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A720" s="1"/>
       <c r="B720" s="12"/>
       <c r="C720" s="12"/>
-      <c r="D720" s="6" t="s">
+      <c r="D720" s="25" t="s">
         <v>1544</v>
       </c>
-      <c r="E720" s="32" t="s">
+      <c r="E720" s="33" t="s">
         <v>1545</v>
       </c>
-      <c r="F720" s="11" t="s">
+      <c r="F720" s="24" t="s">
         <v>1546</v>
       </c>
-    </row>
-    <row r="721" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G720" s="22" t="s">
+        <v>7370</v>
+      </c>
+    </row>
+    <row r="721" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A721" s="1"/>
       <c r="B721" s="12"/>
       <c r="C721" s="12"/>
-      <c r="D721" s="6" t="s">
+      <c r="D721" s="25" t="s">
         <v>1547</v>
       </c>
-      <c r="E721" s="32" t="s">
+      <c r="E721" s="33" t="s">
         <v>1548</v>
       </c>
-      <c r="F721" s="11" t="s">
+      <c r="F721" s="24" t="s">
         <v>1549</v>
       </c>
-    </row>
-    <row r="722" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G721" s="22" t="s">
+        <v>7370</v>
+      </c>
+    </row>
+    <row r="722" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A722" s="1"/>
       <c r="B722" s="12"/>
       <c r="C722" s="12"/>
-      <c r="D722" s="6" t="s">
+      <c r="D722" s="25" t="s">
         <v>1550</v>
       </c>
-      <c r="E722" s="32" t="s">
+      <c r="E722" s="33" t="s">
         <v>1551</v>
       </c>
-      <c r="F722" s="11" t="s">
+      <c r="F722" s="24" t="s">
         <v>1552</v>
       </c>
-    </row>
-    <row r="723" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G722" s="22" t="s">
+        <v>7370</v>
+      </c>
+    </row>
+    <row r="723" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A723" s="1"/>
       <c r="B723" s="12"/>
       <c r="C723" s="12"/>
-      <c r="D723" s="6" t="s">
+      <c r="D723" s="25" t="s">
         <v>1553</v>
       </c>
-      <c r="E723" s="32" t="s">
+      <c r="E723" s="33" t="s">
         <v>1554</v>
       </c>
-      <c r="F723" s="11" t="s">
+      <c r="F723" s="24" t="s">
         <v>1158</v>
       </c>
-    </row>
-    <row r="724" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G723" s="22" t="s">
+        <v>7370</v>
+      </c>
+    </row>
+    <row r="724" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A724" s="1" t="s">
         <v>1555</v>
       </c>
@@ -33650,7 +33775,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="725" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="725" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A725" s="1"/>
       <c r="B725" s="12"/>
       <c r="C725" s="12"/>
@@ -33664,7 +33789,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="726" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="726" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A726" s="1"/>
       <c r="B726" s="12"/>
       <c r="C726" s="12"/>
@@ -33678,7 +33803,7 @@
         <v>1563</v>
       </c>
     </row>
-    <row r="727" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A727" s="1" t="s">
         <v>1564</v>
       </c>
@@ -33692,7 +33817,7 @@
       <c r="E727" s="32"/>
       <c r="F727" s="11"/>
     </row>
-    <row r="728" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A728" s="1" t="s">
         <v>1567</v>
       </c>
@@ -33706,7 +33831,7 @@
       <c r="E728" s="32"/>
       <c r="F728" s="11"/>
     </row>
-    <row r="729" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A729" s="1" t="s">
         <v>1570</v>
       </c>
@@ -33720,7 +33845,7 @@
       <c r="E729" s="32"/>
       <c r="F729" s="11"/>
     </row>
-    <row r="730" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A730" s="1" t="s">
         <v>1572</v>
       </c>
@@ -33734,7 +33859,7 @@
       <c r="E730" s="32"/>
       <c r="F730" s="11"/>
     </row>
-    <row r="731" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A731" s="1" t="s">
         <v>1573</v>
       </c>
@@ -33748,7 +33873,7 @@
       <c r="E731" s="32"/>
       <c r="F731" s="11"/>
     </row>
-    <row r="732" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="732" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A732" s="1" t="s">
         <v>1574</v>
       </c>
@@ -33762,7 +33887,7 @@
       <c r="E732" s="32"/>
       <c r="F732" s="11"/>
     </row>
-    <row r="733" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A733" s="1" t="s">
         <v>1576</v>
       </c>
@@ -33782,7 +33907,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="734" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="734" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A734" s="1" t="s">
         <v>1579</v>
       </c>
@@ -33802,7 +33927,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="735" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="735" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A735" s="1" t="s">
         <v>1582</v>
       </c>
@@ -33822,7 +33947,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="736" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="736" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A736" s="1" t="s">
         <v>1585</v>
       </c>
@@ -74405,8 +74530,14 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G588" r:id="rId1" location="issuecomment-1103016991" display="use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete. Also for now make the parent 'alkene oxidative cleavage' also a child of 'oxidative cleavage' undtil this can be inffered instead"/>
+    <hyperlink ref="G587" r:id="rId2" location="issuecomment-1103016991" display="use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete. Also for now make the parent 'alkene oxidative cleavage' also a child of 'oxidative cleavage' undtil this can be inffered instead"/>
+    <hyperlink ref="G589" r:id="rId3" location="issuecomment-1103016991" display="use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete. Also for now make the parent 'alkene oxidative cleavage' also a child of 'oxidative cleavage' undtil this can be inffered instead"/>
+    <hyperlink ref="G591" r:id="rId4" location="issuecomment-1103016991" display="use RXNO version, as this seems to be more precise, but use MOP:0000708 instead of RXNO:0000344 and make the latter obsolete. Also for now make the parent 'alkene oxidative cleavage' also a child of 'oxidative cleavage' undtil this can be inffered instead"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>